<commit_message>
cadre et pas cadre
</commit_message>
<xml_diff>
--- a/src/main/resources/datasources/angleterre/infoPaieAngleterre.xlsx
+++ b/src/main/resources/datasources/angleterre/infoPaieAngleterre.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\IdeaProjects\projetDintegrationGlobalHumanRessource\src\main\resources\datasources\angleterre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4DB4AAB-55AB-41FE-9B17-7CFDF2AFC4C1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95D785A3-37B0-4054-848F-8781B5A63632}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -436,7 +436,7 @@
   <dimension ref="A1:J58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1111,7 +1111,7 @@
       </c>
       <c r="F21">
         <f ca="1">RANDBETWEEN(1,20)</f>
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="G21">
         <v>101.1</v>
@@ -1173,7 +1173,7 @@
       </c>
       <c r="F23">
         <f t="shared" ref="F23:F58" ca="1" si="0">RANDBETWEEN(1,20)</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G23">
         <v>101.1</v>
@@ -1206,7 +1206,7 @@
       </c>
       <c r="F24">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G24">
         <v>101.1</v>
@@ -1239,7 +1239,7 @@
       </c>
       <c r="F25">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G25">
         <v>101.1</v>
@@ -1272,7 +1272,7 @@
       </c>
       <c r="F26">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G26">
         <v>101.1</v>
@@ -1305,7 +1305,7 @@
       </c>
       <c r="F27">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="G27">
         <v>101.1</v>
@@ -1338,7 +1338,7 @@
       </c>
       <c r="F28">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G28">
         <v>101.1</v>
@@ -1371,7 +1371,7 @@
       </c>
       <c r="F29">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G29">
         <v>101.1</v>
@@ -1404,7 +1404,7 @@
       </c>
       <c r="F30">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="G30">
         <v>101.1</v>
@@ -1437,7 +1437,7 @@
       </c>
       <c r="F31">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="G31">
         <v>101.1</v>
@@ -1470,7 +1470,7 @@
       </c>
       <c r="F32">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="G32">
         <v>101.1</v>
@@ -1503,7 +1503,7 @@
       </c>
       <c r="F33">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="G33">
         <v>101.1</v>
@@ -1536,7 +1536,7 @@
       </c>
       <c r="F34">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G34">
         <v>101.1</v>
@@ -1569,7 +1569,7 @@
       </c>
       <c r="F35">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="G35">
         <v>101.1</v>
@@ -1602,7 +1602,7 @@
       </c>
       <c r="F36">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="G36">
         <v>101.1</v>
@@ -1635,7 +1635,7 @@
       </c>
       <c r="F37">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="G37">
         <v>101.1</v>
@@ -1668,7 +1668,7 @@
       </c>
       <c r="F38">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G38">
         <v>101.1</v>
@@ -1734,7 +1734,7 @@
       </c>
       <c r="F40">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G40">
         <v>101.1</v>
@@ -1767,7 +1767,7 @@
       </c>
       <c r="F41">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="G41">
         <v>101.1</v>
@@ -1800,7 +1800,7 @@
       </c>
       <c r="F42">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G42">
         <v>101.1</v>
@@ -1866,7 +1866,7 @@
       </c>
       <c r="F44">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G44">
         <v>101.1</v>
@@ -1899,7 +1899,7 @@
       </c>
       <c r="F45">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G45">
         <v>101.1</v>
@@ -1932,7 +1932,7 @@
       </c>
       <c r="F46">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="G46">
         <v>101.1</v>
@@ -1965,7 +1965,7 @@
       </c>
       <c r="F47">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="G47">
         <v>101.1</v>
@@ -1998,7 +1998,7 @@
       </c>
       <c r="F48">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G48">
         <v>101.1</v>
@@ -2031,7 +2031,7 @@
       </c>
       <c r="F49">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G49">
         <v>101.1</v>
@@ -2064,7 +2064,7 @@
       </c>
       <c r="F50">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="G50">
         <v>101.1</v>
@@ -2097,7 +2097,7 @@
       </c>
       <c r="F51">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G51">
         <v>101.1</v>
@@ -2130,7 +2130,7 @@
       </c>
       <c r="F52">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G52">
         <v>101.1</v>
@@ -2163,7 +2163,7 @@
       </c>
       <c r="F53">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="G53">
         <v>101.1</v>
@@ -2196,7 +2196,7 @@
       </c>
       <c r="F54">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G54">
         <v>101.1</v>
@@ -2229,7 +2229,7 @@
       </c>
       <c r="F55">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G55">
         <v>101.1</v>
@@ -2262,7 +2262,7 @@
       </c>
       <c r="F56">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="G56">
         <v>101.1</v>
@@ -2295,7 +2295,7 @@
       </c>
       <c r="F57">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G57">
         <v>101.1</v>

</xml_diff>